<commit_message>
AG - Updated and organized the Optimization notebook.
</commit_message>
<xml_diff>
--- a/Battery Optimization/results/Result.xlsx
+++ b/Battery Optimization/results/Result.xlsx
@@ -418,7 +418,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>-3.53</v>
+        <v>66.5</v>
       </c>
     </row>
   </sheetData>
@@ -428,7 +428,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:G121"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -456,56 +456,56 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="2">
-        <v>45656</v>
+        <v>45648</v>
       </c>
       <c r="B2">
-        <v>9571.9966</v>
+        <v>7859.66</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>-9</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>-9</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0.5</v>
+        <v>0.9275</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="2">
-        <v>45656.04166666666</v>
+        <v>45648.04166666666</v>
       </c>
       <c r="B3">
-        <v>9428.0479</v>
+        <v>7764.52</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>-0.47</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>-0.47</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0.5</v>
+        <v>0.95</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="2">
-        <v>45656.08333333334</v>
+        <v>45648.08333333334</v>
       </c>
       <c r="B4">
-        <v>9292.450500000001</v>
+        <v>7775.7</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -517,7 +517,7 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0.5</v>
+        <v>0.95</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -525,10 +525,10 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="2">
-        <v>45656.125</v>
+        <v>45648.125</v>
       </c>
       <c r="B5">
-        <v>9231.072700000001</v>
+        <v>7738.64</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -540,7 +540,7 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0.5</v>
+        <v>0.95</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -548,22 +548,22 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="2">
-        <v>45656.16666666666</v>
+        <v>45648.16666666666</v>
       </c>
       <c r="B6">
-        <v>9244.5748</v>
+        <v>7476.88</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>7.15</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>7.15</v>
       </c>
       <c r="F6">
-        <v>0.5</v>
+        <v>0.5737</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -571,22 +571,22 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="2">
-        <v>45656.20833333334</v>
+        <v>45648.20833333334</v>
       </c>
       <c r="B7">
-        <v>9500.235500000001</v>
+        <v>7480.84</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F7">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -594,56 +594,56 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="2">
-        <v>45656.25</v>
+        <v>45648.25</v>
       </c>
       <c r="B8">
-        <v>9740.951499999999</v>
+        <v>7662.47</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>-8.890000000000001</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>-8.890000000000001</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
-        <v>0.5</v>
+        <v>0.5225</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="2">
-        <v>45656.29166666666</v>
+        <v>45648.29166666666</v>
       </c>
       <c r="B9">
-        <v>10095.5059</v>
+        <v>7816.01</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>-9</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>-9</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
-        <v>0.5</v>
+        <v>0.95</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="2">
-        <v>45656.33333333334</v>
+        <v>45648.33333333334</v>
       </c>
       <c r="B10">
-        <v>10380.2987</v>
+        <v>8095.05</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -655,7 +655,7 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>0.5</v>
+        <v>0.95</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -663,22 +663,22 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="2">
-        <v>45656.375</v>
+        <v>45648.375</v>
       </c>
       <c r="B11">
-        <v>10383.9907</v>
+        <v>8361.110000000001</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F11">
-        <v>0.5</v>
+        <v>0.4763</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -686,45 +686,45 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="2">
-        <v>45656.41666666666</v>
+        <v>45648.41666666666</v>
       </c>
       <c r="B12">
-        <v>10378.3625</v>
+        <v>8714.9</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>-2.05</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>-2.05</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12">
-        <v>0.5</v>
+        <v>0.5737</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="2">
-        <v>45656.45833333334</v>
+        <v>45648.45833333334</v>
       </c>
       <c r="B13">
-        <v>10338.5721</v>
+        <v>8642.85</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F13">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -732,10 +732,10 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="2">
-        <v>45656.5</v>
+        <v>45648.5</v>
       </c>
       <c r="B14">
-        <v>10149.0694</v>
+        <v>8560.77</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -747,7 +747,7 @@
         <v>0</v>
       </c>
       <c r="F14">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -755,56 +755,56 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="2">
-        <v>45656.54166666666</v>
+        <v>45648.54166666666</v>
       </c>
       <c r="B15">
-        <v>10094.6495</v>
+        <v>8435.129999999999</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>-8.890000000000001</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>-8.890000000000001</v>
       </c>
       <c r="E15">
         <v>0</v>
       </c>
       <c r="F15">
-        <v>0.5</v>
+        <v>0.5225</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="2">
-        <v>45656.58333333334</v>
+        <v>45648.58333333334</v>
       </c>
       <c r="B16">
-        <v>10211.605</v>
+        <v>8500.85</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>-9</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>-9</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="F16">
-        <v>0.5</v>
+        <v>0.95</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="2">
-        <v>45656.625</v>
+        <v>45648.625</v>
       </c>
       <c r="B17">
-        <v>10452.7262</v>
+        <v>9259.34</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -816,7 +816,7 @@
         <v>0</v>
       </c>
       <c r="F17">
-        <v>0.5</v>
+        <v>0.95</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -824,22 +824,22 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="2">
-        <v>45656.66666666666</v>
+        <v>45648.66666666666</v>
       </c>
       <c r="B18">
-        <v>10855.8783</v>
+        <v>10032</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>7.15</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>7.15</v>
       </c>
       <c r="F18">
-        <v>0.5</v>
+        <v>0.5737</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -847,22 +847,22 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="2">
-        <v>45656.70833333334</v>
+        <v>45648.70833333334</v>
       </c>
       <c r="B19">
-        <v>11078.2326</v>
+        <v>10256.82</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F19">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -870,10 +870,10 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="2">
-        <v>45656.75</v>
+        <v>45648.75</v>
       </c>
       <c r="B20">
-        <v>10905.0074</v>
+        <v>10104.87</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -885,7 +885,7 @@
         <v>0</v>
       </c>
       <c r="F20">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -893,10 +893,10 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="2">
-        <v>45656.79166666666</v>
+        <v>45648.79166666666</v>
       </c>
       <c r="B21">
-        <v>10808.7606</v>
+        <v>9774.58</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -908,7 +908,7 @@
         <v>0</v>
       </c>
       <c r="F21">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -916,10 +916,10 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="2">
-        <v>45656.83333333334</v>
+        <v>45648.83333333334</v>
       </c>
       <c r="B22">
-        <v>10691.513</v>
+        <v>9188.889999999999</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -931,7 +931,7 @@
         <v>0</v>
       </c>
       <c r="F22">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -939,10 +939,10 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="2">
-        <v>45656.875</v>
+        <v>45648.875</v>
       </c>
       <c r="B23">
-        <v>10602.6749</v>
+        <v>8780.370000000001</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -954,7 +954,7 @@
         <v>0</v>
       </c>
       <c r="F23">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -962,10 +962,10 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="2">
-        <v>45656.91666666666</v>
+        <v>45648.91666666666</v>
       </c>
       <c r="B24">
-        <v>10306.551</v>
+        <v>8204.92</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -977,7 +977,7 @@
         <v>0</v>
       </c>
       <c r="F24">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="G24">
         <v>0</v>
@@ -985,10 +985,10 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="2">
-        <v>45656.95833333334</v>
+        <v>45648.95833333334</v>
       </c>
       <c r="B25">
-        <v>10097.8962</v>
+        <v>7753.13</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -1000,7 +1000,7 @@
         <v>0</v>
       </c>
       <c r="F25">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="G25">
         <v>0</v>
@@ -1008,10 +1008,10 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="2">
-        <v>45657</v>
+        <v>45649</v>
       </c>
       <c r="B26">
-        <v>9909.7978</v>
+        <v>7224.97</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -1023,7 +1023,7 @@
         <v>0</v>
       </c>
       <c r="F26">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="G26">
         <v>0</v>
@@ -1031,10 +1031,10 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="2">
-        <v>45657.04166666666</v>
+        <v>45649.04166666666</v>
       </c>
       <c r="B27">
-        <v>9809.7564</v>
+        <v>7073.07</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -1046,7 +1046,7 @@
         <v>0</v>
       </c>
       <c r="F27">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="G27">
         <v>0</v>
@@ -1054,10 +1054,10 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="2">
-        <v>45657.08333333334</v>
+        <v>45649.08333333334</v>
       </c>
       <c r="B28">
-        <v>9822.4666</v>
+        <v>7126.05</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -1069,7 +1069,7 @@
         <v>0</v>
       </c>
       <c r="F28">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="G28">
         <v>0</v>
@@ -1077,10 +1077,10 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="2">
-        <v>45657.125</v>
+        <v>45649.125</v>
       </c>
       <c r="B29">
-        <v>9830.497100000001</v>
+        <v>7054.65</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -1092,7 +1092,7 @@
         <v>0</v>
       </c>
       <c r="F29">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="G29">
         <v>0</v>
@@ -1100,56 +1100,56 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="2">
-        <v>45657.16666666666</v>
+        <v>45649.16666666666</v>
       </c>
       <c r="B30">
-        <v>9896.0656</v>
+        <v>7041.81</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>-8.890000000000001</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>-8.890000000000001</v>
       </c>
       <c r="E30">
         <v>0</v>
       </c>
       <c r="F30">
-        <v>0.5</v>
+        <v>0.5225</v>
       </c>
       <c r="G30">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="2">
-        <v>45657.20833333334</v>
+        <v>45649.20833333334</v>
       </c>
       <c r="B31">
-        <v>10005.9801</v>
+        <v>7088.83</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>-9</v>
       </c>
       <c r="D31">
-        <v>0</v>
+        <v>-9</v>
       </c>
       <c r="E31">
         <v>0</v>
       </c>
       <c r="F31">
-        <v>0.5</v>
+        <v>0.95</v>
       </c>
       <c r="G31">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="2">
-        <v>45657.25</v>
+        <v>45649.25</v>
       </c>
       <c r="B32">
-        <v>10222.7342</v>
+        <v>7185.41</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -1161,7 +1161,7 @@
         <v>0</v>
       </c>
       <c r="F32">
-        <v>0.5</v>
+        <v>0.95</v>
       </c>
       <c r="G32">
         <v>0</v>
@@ -1169,10 +1169,10 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="2">
-        <v>45657.29166666666</v>
+        <v>45649.29166666666</v>
       </c>
       <c r="B33">
-        <v>10544.6028</v>
+        <v>7490.46</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -1184,7 +1184,7 @@
         <v>0</v>
       </c>
       <c r="F33">
-        <v>0.5</v>
+        <v>0.95</v>
       </c>
       <c r="G33">
         <v>0</v>
@@ -1192,22 +1192,22 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="2">
-        <v>45657.33333333334</v>
+        <v>45649.33333333334</v>
       </c>
       <c r="B34">
-        <v>10867.0347</v>
+        <v>8032.14</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D34">
         <v>0</v>
       </c>
       <c r="E34">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F34">
-        <v>0.5</v>
+        <v>0.4763</v>
       </c>
       <c r="G34">
         <v>0</v>
@@ -1215,22 +1215,22 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="2">
-        <v>45657.375</v>
+        <v>45649.375</v>
       </c>
       <c r="B35">
-        <v>10944.243</v>
+        <v>8071.06</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>7.15</v>
       </c>
       <c r="D35">
         <v>0</v>
       </c>
       <c r="E35">
-        <v>0</v>
+        <v>7.15</v>
       </c>
       <c r="F35">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="G35">
         <v>0</v>
@@ -1238,10 +1238,10 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="2">
-        <v>45657.41666666666</v>
+        <v>45649.41666666666</v>
       </c>
       <c r="B36">
-        <v>11068.2613</v>
+        <v>7857.26</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -1253,7 +1253,7 @@
         <v>0</v>
       </c>
       <c r="F36">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="G36">
         <v>0</v>
@@ -1261,19 +1261,19 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="2">
-        <v>45657.45833333334</v>
+        <v>45649.45833333334</v>
       </c>
       <c r="B37">
-        <v>11098.4217</v>
+        <v>7545.6</v>
       </c>
       <c r="C37">
-        <v>7.6</v>
+        <v>0</v>
       </c>
       <c r="D37">
         <v>0</v>
       </c>
       <c r="E37">
-        <v>7.6</v>
+        <v>0</v>
       </c>
       <c r="F37">
         <v>0.1</v>
@@ -1284,10 +1284,10 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="2">
-        <v>45657.5</v>
+        <v>45649.5</v>
       </c>
       <c r="B38">
-        <v>11137.8841</v>
+        <v>6973.69</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -1307,56 +1307,56 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="2">
-        <v>45657.54166666666</v>
+        <v>45649.54166666666</v>
       </c>
       <c r="B39">
-        <v>11136.5503</v>
+        <v>6898.07</v>
       </c>
       <c r="C39">
-        <v>0</v>
+        <v>-9</v>
       </c>
       <c r="D39">
-        <v>0</v>
+        <v>-9</v>
       </c>
       <c r="E39">
         <v>0</v>
       </c>
       <c r="F39">
-        <v>0.1</v>
+        <v>0.5275</v>
       </c>
       <c r="G39">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="2">
-        <v>45657.58333333334</v>
+        <v>45649.58333333334</v>
       </c>
       <c r="B40">
-        <v>11116.0699</v>
+        <v>7025.58</v>
       </c>
       <c r="C40">
-        <v>0</v>
+        <v>-8.890000000000001</v>
       </c>
       <c r="D40">
-        <v>0</v>
+        <v>-8.890000000000001</v>
       </c>
       <c r="E40">
         <v>0</v>
       </c>
       <c r="F40">
-        <v>0.1</v>
+        <v>0.95</v>
       </c>
       <c r="G40">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="2">
-        <v>45657.625</v>
+        <v>45649.625</v>
       </c>
       <c r="B41">
-        <v>11134.3407</v>
+        <v>7505.69</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -1368,7 +1368,7 @@
         <v>0</v>
       </c>
       <c r="F41">
-        <v>0.1</v>
+        <v>0.95</v>
       </c>
       <c r="G41">
         <v>0</v>
@@ -1376,10 +1376,10 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="2">
-        <v>45657.66666666666</v>
+        <v>45649.66666666666</v>
       </c>
       <c r="B42">
-        <v>11286.8963</v>
+        <v>8087.01</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -1391,7 +1391,7 @@
         <v>0</v>
       </c>
       <c r="F42">
-        <v>0.1</v>
+        <v>0.95</v>
       </c>
       <c r="G42">
         <v>0</v>
@@ -1399,22 +1399,22 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="2">
-        <v>45657.70833333334</v>
+        <v>45649.70833333334</v>
       </c>
       <c r="B43">
-        <v>11372.3966</v>
+        <v>8401.74</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>7.15</v>
       </c>
       <c r="D43">
         <v>0</v>
       </c>
       <c r="E43">
-        <v>0</v>
+        <v>7.15</v>
       </c>
       <c r="F43">
-        <v>0.1</v>
+        <v>0.5737</v>
       </c>
       <c r="G43">
         <v>0</v>
@@ -1422,19 +1422,19 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="2">
-        <v>45657.75</v>
+        <v>45649.75</v>
       </c>
       <c r="B44">
-        <v>11019.8642</v>
+        <v>8440.690000000001</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D44">
         <v>0</v>
       </c>
       <c r="E44">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F44">
         <v>0.1</v>
@@ -1445,56 +1445,56 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="2">
-        <v>45657.79166666666</v>
+        <v>45649.79166666666</v>
       </c>
       <c r="B45">
-        <v>10789.3804</v>
+        <v>8362.17</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>-9</v>
       </c>
       <c r="D45">
-        <v>0</v>
+        <v>-9</v>
       </c>
       <c r="E45">
         <v>0</v>
       </c>
       <c r="F45">
-        <v>0.1</v>
+        <v>0.5275</v>
       </c>
       <c r="G45">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="2">
-        <v>45657.83333333334</v>
+        <v>45649.83333333334</v>
       </c>
       <c r="B46">
-        <v>10661.5569</v>
+        <v>8417.190000000001</v>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>-8.890000000000001</v>
       </c>
       <c r="D46">
-        <v>0</v>
+        <v>-8.890000000000001</v>
       </c>
       <c r="E46">
         <v>0</v>
       </c>
       <c r="F46">
-        <v>0.1</v>
+        <v>0.95</v>
       </c>
       <c r="G46">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="2">
-        <v>45657.875</v>
+        <v>45649.875</v>
       </c>
       <c r="B47">
-        <v>10576.2663</v>
+        <v>8686.27</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -1506,7 +1506,7 @@
         <v>0</v>
       </c>
       <c r="F47">
-        <v>0.1</v>
+        <v>0.95</v>
       </c>
       <c r="G47">
         <v>0</v>
@@ -1514,22 +1514,22 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="2">
-        <v>45657.91666666666</v>
+        <v>45649.91666666666</v>
       </c>
       <c r="B48">
-        <v>10420.67</v>
+        <v>8890.99</v>
       </c>
       <c r="C48">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D48">
         <v>0</v>
       </c>
       <c r="E48">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F48">
-        <v>0.1</v>
+        <v>0.4763</v>
       </c>
       <c r="G48">
         <v>0</v>
@@ -1537,24 +1537,1680 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="2">
-        <v>45657.95833333334</v>
+        <v>45649.95833333334</v>
       </c>
       <c r="B49">
-        <v>10280.1889</v>
+        <v>8804.030000000001</v>
       </c>
       <c r="C49">
-        <v>0</v>
+        <v>-9</v>
       </c>
       <c r="D49">
-        <v>0</v>
+        <v>-9</v>
       </c>
       <c r="E49">
         <v>0</v>
       </c>
       <c r="F49">
-        <v>0.1</v>
+        <v>0.9038</v>
       </c>
       <c r="G49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="2">
+        <v>45650</v>
+      </c>
+      <c r="B50">
+        <v>8890.59</v>
+      </c>
+      <c r="C50">
+        <v>6.27</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>6.27</v>
+      </c>
+      <c r="F50">
+        <v>0.5737</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="2">
+        <v>45650.04166666666</v>
+      </c>
+      <c r="B51">
+        <v>9099.290000000001</v>
+      </c>
+      <c r="C51">
+        <v>9</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>9</v>
+      </c>
+      <c r="F51">
+        <v>0.1</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="2">
+        <v>45650.08333333334</v>
+      </c>
+      <c r="B52">
+        <v>8714.940000000001</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52">
+        <v>0.1</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" s="2">
+        <v>45650.125</v>
+      </c>
+      <c r="B53">
+        <v>8172.04</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>0.1</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" s="2">
+        <v>45650.16666666666</v>
+      </c>
+      <c r="B54">
+        <v>7778.06</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>0.1</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" s="2">
+        <v>45650.20833333334</v>
+      </c>
+      <c r="B55">
+        <v>7667.69</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>0.1</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" s="2">
+        <v>45650.25</v>
+      </c>
+      <c r="B56">
+        <v>7538.52</v>
+      </c>
+      <c r="C56">
+        <v>-0.97</v>
+      </c>
+      <c r="D56">
+        <v>-0.97</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>0.1462</v>
+      </c>
+      <c r="G56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" s="2">
+        <v>45650.29166666666</v>
+      </c>
+      <c r="B57">
+        <v>7572.83</v>
+      </c>
+      <c r="C57">
+        <v>-9</v>
+      </c>
+      <c r="D57">
+        <v>-9</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>0.5737</v>
+      </c>
+      <c r="G57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" s="2">
+        <v>45650.33333333334</v>
+      </c>
+      <c r="B58">
+        <v>7902.4</v>
+      </c>
+      <c r="C58">
+        <v>9</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>9</v>
+      </c>
+      <c r="F58">
+        <v>0.1</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" s="2">
+        <v>45650.375</v>
+      </c>
+      <c r="B59">
+        <v>7716.2</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <v>0.1</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" s="2">
+        <v>45650.41666666666</v>
+      </c>
+      <c r="B60">
+        <v>7641.1</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <v>0.1</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" s="2">
+        <v>45650.45833333334</v>
+      </c>
+      <c r="B61">
+        <v>7308.09</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>0.1</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" s="2">
+        <v>45650.5</v>
+      </c>
+      <c r="B62">
+        <v>7074.87</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>0.1</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" s="2">
+        <v>45650.54166666666</v>
+      </c>
+      <c r="B63">
+        <v>7054.43</v>
+      </c>
+      <c r="C63">
+        <v>-8.890000000000001</v>
+      </c>
+      <c r="D63">
+        <v>-8.890000000000001</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <v>0.5225</v>
+      </c>
+      <c r="G63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" s="2">
+        <v>45650.58333333334</v>
+      </c>
+      <c r="B64">
+        <v>7000.89</v>
+      </c>
+      <c r="C64">
+        <v>-9</v>
+      </c>
+      <c r="D64">
+        <v>-9</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <v>0.95</v>
+      </c>
+      <c r="G64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" s="2">
+        <v>45650.625</v>
+      </c>
+      <c r="B65">
+        <v>7175.73</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>0.95</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" s="2">
+        <v>45650.66666666666</v>
+      </c>
+      <c r="B66">
+        <v>7642.21</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66">
+        <v>0.95</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67" s="2">
+        <v>45650.70833333334</v>
+      </c>
+      <c r="B67">
+        <v>7773.59</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67">
+        <v>0.95</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" s="2">
+        <v>45650.75</v>
+      </c>
+      <c r="B68">
+        <v>7752.96</v>
+      </c>
+      <c r="C68">
+        <v>7.15</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <v>7.15</v>
+      </c>
+      <c r="F68">
+        <v>0.5737</v>
+      </c>
+      <c r="G68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" s="2">
+        <v>45650.79166666666</v>
+      </c>
+      <c r="B69">
+        <v>7803.81</v>
+      </c>
+      <c r="C69">
+        <v>9</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69">
+        <v>9</v>
+      </c>
+      <c r="F69">
+        <v>0.1</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70" s="2">
+        <v>45650.83333333334</v>
+      </c>
+      <c r="B70">
+        <v>7713.32</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <v>0.1</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71" s="2">
+        <v>45650.875</v>
+      </c>
+      <c r="B71">
+        <v>7356.61</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71">
+        <v>0.1</v>
+      </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72" s="2">
+        <v>45650.91666666666</v>
+      </c>
+      <c r="B72">
+        <v>7123.39</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <v>0.1</v>
+      </c>
+      <c r="G72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="A73" s="2">
+        <v>45650.95833333334</v>
+      </c>
+      <c r="B73">
+        <v>6923.06</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73">
+        <v>0.1</v>
+      </c>
+      <c r="G73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="A74" s="2">
+        <v>45651</v>
+      </c>
+      <c r="B74">
+        <v>6794.22</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74">
+        <v>0.1</v>
+      </c>
+      <c r="G74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="A75" s="2">
+        <v>45651.04166666666</v>
+      </c>
+      <c r="B75">
+        <v>6832.53</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="F75">
+        <v>0.1</v>
+      </c>
+      <c r="G75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
+      <c r="A76" s="2">
+        <v>45651.08333333334</v>
+      </c>
+      <c r="B76">
+        <v>6840.18</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+      <c r="F76">
+        <v>0.1</v>
+      </c>
+      <c r="G76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="A77" s="2">
+        <v>45651.125</v>
+      </c>
+      <c r="B77">
+        <v>6862.94</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77">
+        <v>0</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+      <c r="F77">
+        <v>0.1</v>
+      </c>
+      <c r="G77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="A78" s="2">
+        <v>45651.16666666666</v>
+      </c>
+      <c r="B78">
+        <v>6927.7</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78">
+        <v>0</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
+      </c>
+      <c r="F78">
+        <v>0.1</v>
+      </c>
+      <c r="G78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="A79" s="2">
+        <v>45651.20833333334</v>
+      </c>
+      <c r="B79">
+        <v>6940.13</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
+      </c>
+      <c r="D79">
+        <v>0</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+      <c r="F79">
+        <v>0.1</v>
+      </c>
+      <c r="G79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="A80" s="2">
+        <v>45651.25</v>
+      </c>
+      <c r="B80">
+        <v>6937.12</v>
+      </c>
+      <c r="C80">
+        <v>-8.890000000000001</v>
+      </c>
+      <c r="D80">
+        <v>-8.890000000000001</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+      <c r="F80">
+        <v>0.5225</v>
+      </c>
+      <c r="G80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
+      <c r="A81" s="2">
+        <v>45651.29166666666</v>
+      </c>
+      <c r="B81">
+        <v>6964.68</v>
+      </c>
+      <c r="C81">
+        <v>-9</v>
+      </c>
+      <c r="D81">
+        <v>-9</v>
+      </c>
+      <c r="E81">
+        <v>0</v>
+      </c>
+      <c r="F81">
+        <v>0.95</v>
+      </c>
+      <c r="G81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
+      <c r="A82" s="2">
+        <v>45651.33333333334</v>
+      </c>
+      <c r="B82">
+        <v>6962.76</v>
+      </c>
+      <c r="C82">
+        <v>9</v>
+      </c>
+      <c r="D82">
+        <v>0</v>
+      </c>
+      <c r="E82">
+        <v>9</v>
+      </c>
+      <c r="F82">
+        <v>0.4763</v>
+      </c>
+      <c r="G82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
+      <c r="A83" s="2">
+        <v>45651.375</v>
+      </c>
+      <c r="B83">
+        <v>6885.18</v>
+      </c>
+      <c r="C83">
+        <v>-0.97</v>
+      </c>
+      <c r="D83">
+        <v>-0.97</v>
+      </c>
+      <c r="E83">
+        <v>0</v>
+      </c>
+      <c r="F83">
+        <v>0.5225</v>
+      </c>
+      <c r="G83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
+      <c r="A84" s="2">
+        <v>45651.41666666666</v>
+      </c>
+      <c r="B84">
+        <v>6963.82</v>
+      </c>
+      <c r="C84">
+        <v>-9</v>
+      </c>
+      <c r="D84">
+        <v>-9</v>
+      </c>
+      <c r="E84">
+        <v>0</v>
+      </c>
+      <c r="F84">
+        <v>0.95</v>
+      </c>
+      <c r="G84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
+      <c r="A85" s="2">
+        <v>45651.45833333334</v>
+      </c>
+      <c r="B85">
+        <v>7035.35</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+      <c r="E85">
+        <v>0</v>
+      </c>
+      <c r="F85">
+        <v>0.95</v>
+      </c>
+      <c r="G85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
+      <c r="A86" s="2">
+        <v>45651.5</v>
+      </c>
+      <c r="B86">
+        <v>7084.77</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
+      </c>
+      <c r="D86">
+        <v>0</v>
+      </c>
+      <c r="E86">
+        <v>0</v>
+      </c>
+      <c r="F86">
+        <v>0.95</v>
+      </c>
+      <c r="G86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
+      <c r="A87" s="2">
+        <v>45651.54166666666</v>
+      </c>
+      <c r="B87">
+        <v>7164.26</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="D87">
+        <v>0</v>
+      </c>
+      <c r="E87">
+        <v>0</v>
+      </c>
+      <c r="F87">
+        <v>0.95</v>
+      </c>
+      <c r="G87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
+      <c r="A88" s="2">
+        <v>45651.58333333334</v>
+      </c>
+      <c r="B88">
+        <v>7488.95</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
+      <c r="E88">
+        <v>0</v>
+      </c>
+      <c r="F88">
+        <v>0.95</v>
+      </c>
+      <c r="G88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
+      <c r="A89" s="2">
+        <v>45651.625</v>
+      </c>
+      <c r="B89">
+        <v>8168.43</v>
+      </c>
+      <c r="C89">
+        <v>7.15</v>
+      </c>
+      <c r="D89">
+        <v>0</v>
+      </c>
+      <c r="E89">
+        <v>7.15</v>
+      </c>
+      <c r="F89">
+        <v>0.5737</v>
+      </c>
+      <c r="G89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
+      <c r="A90" s="2">
+        <v>45651.66666666666</v>
+      </c>
+      <c r="B90">
+        <v>8218.33</v>
+      </c>
+      <c r="C90">
+        <v>9</v>
+      </c>
+      <c r="D90">
+        <v>0</v>
+      </c>
+      <c r="E90">
+        <v>9</v>
+      </c>
+      <c r="F90">
+        <v>0.1</v>
+      </c>
+      <c r="G90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
+      <c r="A91" s="2">
+        <v>45651.70833333334</v>
+      </c>
+      <c r="B91">
+        <v>7540.28</v>
+      </c>
+      <c r="C91">
+        <v>0</v>
+      </c>
+      <c r="D91">
+        <v>0</v>
+      </c>
+      <c r="E91">
+        <v>0</v>
+      </c>
+      <c r="F91">
+        <v>0.1</v>
+      </c>
+      <c r="G91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
+      <c r="A92" s="2">
+        <v>45651.75</v>
+      </c>
+      <c r="B92">
+        <v>6952.04</v>
+      </c>
+      <c r="C92">
+        <v>0</v>
+      </c>
+      <c r="D92">
+        <v>0</v>
+      </c>
+      <c r="E92">
+        <v>0</v>
+      </c>
+      <c r="F92">
+        <v>0.1</v>
+      </c>
+      <c r="G92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
+      <c r="A93" s="2">
+        <v>45651.79166666666</v>
+      </c>
+      <c r="B93">
+        <v>6979.77</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+      <c r="E93">
+        <v>0</v>
+      </c>
+      <c r="F93">
+        <v>0.1</v>
+      </c>
+      <c r="G93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
+      <c r="A94" s="2">
+        <v>45651.83333333334</v>
+      </c>
+      <c r="B94">
+        <v>7020.24</v>
+      </c>
+      <c r="C94">
+        <v>0</v>
+      </c>
+      <c r="D94">
+        <v>0</v>
+      </c>
+      <c r="E94">
+        <v>0</v>
+      </c>
+      <c r="F94">
+        <v>0.1</v>
+      </c>
+      <c r="G94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
+      <c r="A95" s="2">
+        <v>45651.875</v>
+      </c>
+      <c r="B95">
+        <v>7012.18</v>
+      </c>
+      <c r="C95">
+        <v>0</v>
+      </c>
+      <c r="D95">
+        <v>0</v>
+      </c>
+      <c r="E95">
+        <v>0</v>
+      </c>
+      <c r="F95">
+        <v>0.1</v>
+      </c>
+      <c r="G95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
+      <c r="A96" s="2">
+        <v>45651.91666666666</v>
+      </c>
+      <c r="B96">
+        <v>6896.49</v>
+      </c>
+      <c r="C96">
+        <v>0</v>
+      </c>
+      <c r="D96">
+        <v>0</v>
+      </c>
+      <c r="E96">
+        <v>0</v>
+      </c>
+      <c r="F96">
+        <v>0.1</v>
+      </c>
+      <c r="G96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7">
+      <c r="A97" s="2">
+        <v>45651.95833333334</v>
+      </c>
+      <c r="B97">
+        <v>6879.49</v>
+      </c>
+      <c r="C97">
+        <v>0</v>
+      </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+      <c r="E97">
+        <v>0</v>
+      </c>
+      <c r="F97">
+        <v>0.1</v>
+      </c>
+      <c r="G97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7">
+      <c r="A98" s="2">
+        <v>45652</v>
+      </c>
+      <c r="B98">
+        <v>7032.07</v>
+      </c>
+      <c r="C98">
+        <v>0</v>
+      </c>
+      <c r="D98">
+        <v>0</v>
+      </c>
+      <c r="E98">
+        <v>0</v>
+      </c>
+      <c r="F98">
+        <v>0.1</v>
+      </c>
+      <c r="G98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7">
+      <c r="A99" s="2">
+        <v>45652.04166666666</v>
+      </c>
+      <c r="B99">
+        <v>7318.81</v>
+      </c>
+      <c r="C99">
+        <v>0</v>
+      </c>
+      <c r="D99">
+        <v>0</v>
+      </c>
+      <c r="E99">
+        <v>0</v>
+      </c>
+      <c r="F99">
+        <v>0.1</v>
+      </c>
+      <c r="G99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7">
+      <c r="A100" s="2">
+        <v>45652.08333333334</v>
+      </c>
+      <c r="B100">
+        <v>7361.03</v>
+      </c>
+      <c r="C100">
+        <v>0</v>
+      </c>
+      <c r="D100">
+        <v>0</v>
+      </c>
+      <c r="E100">
+        <v>0</v>
+      </c>
+      <c r="F100">
+        <v>0.1</v>
+      </c>
+      <c r="G100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7">
+      <c r="A101" s="2">
+        <v>45652.125</v>
+      </c>
+      <c r="B101">
+        <v>7363.69</v>
+      </c>
+      <c r="C101">
+        <v>0</v>
+      </c>
+      <c r="D101">
+        <v>0</v>
+      </c>
+      <c r="E101">
+        <v>0</v>
+      </c>
+      <c r="F101">
+        <v>0.1</v>
+      </c>
+      <c r="G101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7">
+      <c r="A102" s="2">
+        <v>45652.16666666666</v>
+      </c>
+      <c r="B102">
+        <v>7368.78</v>
+      </c>
+      <c r="C102">
+        <v>-8.890000000000001</v>
+      </c>
+      <c r="D102">
+        <v>-8.890000000000001</v>
+      </c>
+      <c r="E102">
+        <v>0</v>
+      </c>
+      <c r="F102">
+        <v>0.5225</v>
+      </c>
+      <c r="G102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7">
+      <c r="A103" s="2">
+        <v>45652.20833333334</v>
+      </c>
+      <c r="B103">
+        <v>7450.6</v>
+      </c>
+      <c r="C103">
+        <v>-9</v>
+      </c>
+      <c r="D103">
+        <v>-9</v>
+      </c>
+      <c r="E103">
+        <v>0</v>
+      </c>
+      <c r="F103">
+        <v>0.95</v>
+      </c>
+      <c r="G103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7">
+      <c r="A104" s="2">
+        <v>45652.25</v>
+      </c>
+      <c r="B104">
+        <v>7505.32</v>
+      </c>
+      <c r="C104">
+        <v>0</v>
+      </c>
+      <c r="D104">
+        <v>0</v>
+      </c>
+      <c r="E104">
+        <v>0</v>
+      </c>
+      <c r="F104">
+        <v>0.95</v>
+      </c>
+      <c r="G104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7">
+      <c r="A105" s="2">
+        <v>45652.29166666666</v>
+      </c>
+      <c r="B105">
+        <v>7598.7</v>
+      </c>
+      <c r="C105">
+        <v>0</v>
+      </c>
+      <c r="D105">
+        <v>0</v>
+      </c>
+      <c r="E105">
+        <v>0</v>
+      </c>
+      <c r="F105">
+        <v>0.95</v>
+      </c>
+      <c r="G105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7">
+      <c r="A106" s="2">
+        <v>45652.33333333334</v>
+      </c>
+      <c r="B106">
+        <v>8094.7</v>
+      </c>
+      <c r="C106">
+        <v>0</v>
+      </c>
+      <c r="D106">
+        <v>0</v>
+      </c>
+      <c r="E106">
+        <v>0</v>
+      </c>
+      <c r="F106">
+        <v>0.95</v>
+      </c>
+      <c r="G106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7">
+      <c r="A107" s="2">
+        <v>45652.375</v>
+      </c>
+      <c r="B107">
+        <v>8405.620000000001</v>
+      </c>
+      <c r="C107">
+        <v>0</v>
+      </c>
+      <c r="D107">
+        <v>0</v>
+      </c>
+      <c r="E107">
+        <v>0</v>
+      </c>
+      <c r="F107">
+        <v>0.95</v>
+      </c>
+      <c r="G107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7">
+      <c r="A108" s="2">
+        <v>45652.41666666666</v>
+      </c>
+      <c r="B108">
+        <v>8708.690000000001</v>
+      </c>
+      <c r="C108">
+        <v>0</v>
+      </c>
+      <c r="D108">
+        <v>0</v>
+      </c>
+      <c r="E108">
+        <v>0</v>
+      </c>
+      <c r="F108">
+        <v>0.95</v>
+      </c>
+      <c r="G108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7">
+      <c r="A109" s="2">
+        <v>45652.45833333334</v>
+      </c>
+      <c r="B109">
+        <v>8830.040000000001</v>
+      </c>
+      <c r="C109">
+        <v>0</v>
+      </c>
+      <c r="D109">
+        <v>0</v>
+      </c>
+      <c r="E109">
+        <v>0</v>
+      </c>
+      <c r="F109">
+        <v>0.95</v>
+      </c>
+      <c r="G109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7">
+      <c r="A110" s="2">
+        <v>45652.5</v>
+      </c>
+      <c r="B110">
+        <v>8835.280000000001</v>
+      </c>
+      <c r="C110">
+        <v>0</v>
+      </c>
+      <c r="D110">
+        <v>0</v>
+      </c>
+      <c r="E110">
+        <v>0</v>
+      </c>
+      <c r="F110">
+        <v>0.95</v>
+      </c>
+      <c r="G110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7">
+      <c r="A111" s="2">
+        <v>45652.54166666666</v>
+      </c>
+      <c r="B111">
+        <v>8788.83</v>
+      </c>
+      <c r="C111">
+        <v>0</v>
+      </c>
+      <c r="D111">
+        <v>0</v>
+      </c>
+      <c r="E111">
+        <v>0</v>
+      </c>
+      <c r="F111">
+        <v>0.95</v>
+      </c>
+      <c r="G111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7">
+      <c r="A112" s="2">
+        <v>45652.58333333334</v>
+      </c>
+      <c r="B112">
+        <v>8863.98</v>
+      </c>
+      <c r="C112">
+        <v>0</v>
+      </c>
+      <c r="D112">
+        <v>0</v>
+      </c>
+      <c r="E112">
+        <v>0</v>
+      </c>
+      <c r="F112">
+        <v>0.95</v>
+      </c>
+      <c r="G112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7">
+      <c r="A113" s="2">
+        <v>45652.625</v>
+      </c>
+      <c r="B113">
+        <v>8829.57</v>
+      </c>
+      <c r="C113">
+        <v>0</v>
+      </c>
+      <c r="D113">
+        <v>0</v>
+      </c>
+      <c r="E113">
+        <v>0</v>
+      </c>
+      <c r="F113">
+        <v>0.95</v>
+      </c>
+      <c r="G113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7">
+      <c r="A114" s="2">
+        <v>45652.66666666666</v>
+      </c>
+      <c r="B114">
+        <v>8974.610000000001</v>
+      </c>
+      <c r="C114">
+        <v>7.15</v>
+      </c>
+      <c r="D114">
+        <v>0</v>
+      </c>
+      <c r="E114">
+        <v>7.15</v>
+      </c>
+      <c r="F114">
+        <v>0.5737</v>
+      </c>
+      <c r="G114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7">
+      <c r="A115" s="2">
+        <v>45652.70833333334</v>
+      </c>
+      <c r="B115">
+        <v>9180.83</v>
+      </c>
+      <c r="C115">
+        <v>9</v>
+      </c>
+      <c r="D115">
+        <v>0</v>
+      </c>
+      <c r="E115">
+        <v>9</v>
+      </c>
+      <c r="F115">
+        <v>0.1</v>
+      </c>
+      <c r="G115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7">
+      <c r="A116" s="2">
+        <v>45652.75</v>
+      </c>
+      <c r="B116">
+        <v>8796.450000000001</v>
+      </c>
+      <c r="C116">
+        <v>0</v>
+      </c>
+      <c r="D116">
+        <v>0</v>
+      </c>
+      <c r="E116">
+        <v>0</v>
+      </c>
+      <c r="F116">
+        <v>0.1</v>
+      </c>
+      <c r="G116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7">
+      <c r="A117" s="2">
+        <v>45652.79166666666</v>
+      </c>
+      <c r="B117">
+        <v>8346.23</v>
+      </c>
+      <c r="C117">
+        <v>-0.97</v>
+      </c>
+      <c r="D117">
+        <v>-0.97</v>
+      </c>
+      <c r="E117">
+        <v>0</v>
+      </c>
+      <c r="F117">
+        <v>0.1462</v>
+      </c>
+      <c r="G117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7">
+      <c r="A118" s="2">
+        <v>45652.83333333334</v>
+      </c>
+      <c r="B118">
+        <v>8212.879999999999</v>
+      </c>
+      <c r="C118">
+        <v>-9</v>
+      </c>
+      <c r="D118">
+        <v>-9</v>
+      </c>
+      <c r="E118">
+        <v>0</v>
+      </c>
+      <c r="F118">
+        <v>0.5737</v>
+      </c>
+      <c r="G118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7">
+      <c r="A119" s="2">
+        <v>45652.875</v>
+      </c>
+      <c r="B119">
+        <v>8025.87</v>
+      </c>
+      <c r="C119">
+        <v>9</v>
+      </c>
+      <c r="D119">
+        <v>0</v>
+      </c>
+      <c r="E119">
+        <v>9</v>
+      </c>
+      <c r="F119">
+        <v>0.1</v>
+      </c>
+      <c r="G119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7">
+      <c r="A120" s="2">
+        <v>45652.91666666666</v>
+      </c>
+      <c r="B120">
+        <v>7771.93</v>
+      </c>
+      <c r="C120">
+        <v>0</v>
+      </c>
+      <c r="D120">
+        <v>0</v>
+      </c>
+      <c r="E120">
+        <v>0</v>
+      </c>
+      <c r="F120">
+        <v>0.1</v>
+      </c>
+      <c r="G120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7">
+      <c r="A121" s="2">
+        <v>45652.95833333334</v>
+      </c>
+      <c r="B121">
+        <v>7509.36</v>
+      </c>
+      <c r="C121">
+        <v>0</v>
+      </c>
+      <c r="D121">
+        <v>0</v>
+      </c>
+      <c r="E121">
+        <v>0</v>
+      </c>
+      <c r="F121">
+        <v>0.1</v>
+      </c>
+      <c r="G121">
         <v>0</v>
       </c>
     </row>

</xml_diff>